<commit_message>
Added graphs & tables to xlsx files
</commit_message>
<xml_diff>
--- a/Lacex_summary_101119_NoT1Lex_0.5.xlsx
+++ b/Lacex_summary_101119_NoT1Lex_0.5.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E77C341-2332-486A-A9DB-426A552A084B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439DDC67-9199-43ED-96F5-305E94546115}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CBF9852-A622-4997-A6B4-FC10C0A9840A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="27">
   <si>
     <t>HK-2</t>
   </si>
@@ -100,6 +101,18 @@
   </si>
   <si>
     <t>RMSE_Lacex</t>
+  </si>
+  <si>
+    <t>4.29E-03 ± 4.51E-04</t>
+  </si>
+  <si>
+    <t>1.24E-04 ± 1.24E-04</t>
+  </si>
+  <si>
+    <t>2.17E-05 ± 2.17E-05</t>
+  </si>
+  <si>
+    <t>6.18E-05 ± 6.18E-05</t>
   </si>
 </sst>
 </file>
@@ -182,16 +195,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -208,6 +221,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -218,6 +242,150 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-619B-4286-AB10-60342F441320}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-619B-4286-AB10-60342F441320}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-619B-4286-AB10-60342F441320}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-619B-4286-AB10-60342F441320}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$C$24:$F$24</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>4.5136714056914323E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.1220074661279486E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.7635577441879949E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.1599662009929656E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$C$24:$F$24</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>4.5136714056914323E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.1220074661279486E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.7635577441879949E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.1599662009929656E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$C$22:$F$22</c:f>
@@ -261,7 +429,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-822C-4BEF-BCF0-C671DA5507F5}"/>
+              <c16:uniqueId val="{00000000-619B-4286-AB10-60342F441320}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -275,11 +443,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="593045496"/>
-        <c:axId val="593046808"/>
+        <c:axId val="436147016"/>
+        <c:axId val="436146032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="593045496"/>
+        <c:axId val="436147016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -307,22 +475,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593046808"/>
+        <c:crossAx val="436146032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -330,7 +498,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="593046808"/>
+        <c:axId val="436146032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -366,22 +534,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="593045496"/>
+        <c:crossAx val="436147016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -424,7 +592,886 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr b="1">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1A5B-4EE6-AC41-016CEA4B6EDC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-1A5B-4EE6-AC41-016CEA4B6EDC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1A5B-4EE6-AC41-016CEA4B6EDC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-1A5B-4EE6-AC41-016CEA4B6EDC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$G$40:$J$40</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.9144315790535879E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.44397388421656619</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.88615526584189808</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.44937654633895496</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$G$40:$J$40</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.9144315790535879E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.44397388421656619</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.88615526584189808</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.44937654633895496</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$G$38:$J$38</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>HK-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UMRC6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UOK262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>UOK + DIDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$39:$J$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.18569186105247851</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90130002426451794</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2736220748081715</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53268202141294263</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1A5B-4EE6-AC41-016CEA4B6EDC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="436153904"/>
+        <c:axId val="436153248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="436153904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="436153248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="436153248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="436153904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr b="1">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T1Lin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B10C-4B36-88C7-F8D3B03EA403}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-B10C-4B36-88C7-F8D3B03EA403}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B10C-4B36-88C7-F8D3B03EA403}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-B10C-4B36-88C7-F8D3B03EA403}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$E$32:$H$32</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>5.5763549867175604</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.4484216607654696</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.038832203919124</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.0195995714306711</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$E$32:$H$32</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>5.5763549867175604</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.4484216607654696</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.038832203919124</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.0195995714306711</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$30:$H$30</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>HK-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UMRC6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UOK262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>UOK262 with DIDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$31:$H$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20.810952355822621</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.729581396574176</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.645077264540124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.226799957017924</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B10C-4B36-88C7-F8D3B03EA403}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="598674760"/>
+        <c:axId val="598676400"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="598674760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="598676400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="598676400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="598674760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr b="1">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -477,7 +1524,1093 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -997,10 +3130,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{131F5732-96E2-43CD-842D-773F213A5122}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9854C348-A373-4F0B-9CED-234671AFDED0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1013,6 +3146,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3E71C1B-E3AB-4AC9-9165-1200AB7D910F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EE082DC-7950-4CC8-9AA3-F37FD2EA7F9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1318,10 +3523,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90DEE466-AA1C-46E8-9053-4DA781462313}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:F23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3814,4 +6020,482 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0018BC78-2323-4789-8891-B2789482A6AA}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>49.301098614300237</v>
+      </c>
+      <c r="C2">
+        <v>4.2896681809653234E-3</v>
+      </c>
+      <c r="D2">
+        <v>0.18960492684311411</v>
+      </c>
+      <c r="E2">
+        <v>20.810952355822621</v>
+      </c>
+      <c r="F2">
+        <v>3.0839808344364923E-14</v>
+      </c>
+      <c r="G2">
+        <v>0.18569186105247851</v>
+      </c>
+      <c r="H2">
+        <v>0.15167392099321886</v>
+      </c>
+      <c r="I2">
+        <v>5.6769502229053331E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>49.562286765310184</v>
+      </c>
+      <c r="C3">
+        <v>2.3214600759283919E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.10071906033659894</v>
+      </c>
+      <c r="E3">
+        <v>19.729581396574176</v>
+      </c>
+      <c r="F3">
+        <v>2.168300617539897E-5</v>
+      </c>
+      <c r="G3">
+        <v>0.90130002426451794</v>
+      </c>
+      <c r="H3">
+        <v>0.80963329111612248</v>
+      </c>
+      <c r="I3">
+        <v>1.2396217176390044E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>50.611708607311165</v>
+      </c>
+      <c r="C4">
+        <v>2.9445341368774566E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.14887617308574641</v>
+      </c>
+      <c r="E4">
+        <v>16.645077264540124</v>
+      </c>
+      <c r="F4">
+        <v>6.1785810751357006E-5</v>
+      </c>
+      <c r="G4">
+        <v>1.2736220748081715</v>
+      </c>
+      <c r="H4">
+        <v>3.3995059350725314</v>
+      </c>
+      <c r="I4">
+        <v>3.5013802233955498E-9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>50.393050399381366</v>
+      </c>
+      <c r="C5">
+        <v>1.717071175865973E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.12554936463342373</v>
+      </c>
+      <c r="E5">
+        <v>17.226799957017924</v>
+      </c>
+      <c r="F5">
+        <v>1.2517235064489362E-2</v>
+      </c>
+      <c r="G5">
+        <v>0.53268202141294263</v>
+      </c>
+      <c r="H5">
+        <v>2.6839364723061769</v>
+      </c>
+      <c r="I5">
+        <v>2.7687596607677895E-14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0.74523230645633032</v>
+      </c>
+      <c r="C8">
+        <v>4.5136714056914323E-4</v>
+      </c>
+      <c r="D8">
+        <v>3.453818284697778E-2</v>
+      </c>
+      <c r="E8">
+        <v>5.5763549867175604</v>
+      </c>
+      <c r="F8">
+        <v>6.8584445626451913E-15</v>
+      </c>
+      <c r="G8">
+        <v>3.9144315790535879E-2</v>
+      </c>
+      <c r="H8">
+        <v>3.9814552957846479E-2</v>
+      </c>
+      <c r="I8">
+        <v>5.6769448457710148E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0.19348725408279632</v>
+      </c>
+      <c r="C9">
+        <v>1.1220074661279486E-2</v>
+      </c>
+      <c r="D9">
+        <v>9.8374746609311503E-2</v>
+      </c>
+      <c r="E9">
+        <v>4.4484216607654696</v>
+      </c>
+      <c r="F9">
+        <v>2.1681951239300393E-5</v>
+      </c>
+      <c r="G9">
+        <v>0.44397388421656619</v>
+      </c>
+      <c r="H9">
+        <v>0.45108212606096143</v>
+      </c>
+      <c r="I9">
+        <v>1.2396202754059109E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0.38820549252012182</v>
+      </c>
+      <c r="C10">
+        <v>1.7635577441879949E-2</v>
+      </c>
+      <c r="D10">
+        <v>7.0123337535262342E-2</v>
+      </c>
+      <c r="E10">
+        <v>3.038832203919124</v>
+      </c>
+      <c r="F10">
+        <v>6.1785810715830547E-5</v>
+      </c>
+      <c r="G10">
+        <v>0.88615526584189808</v>
+      </c>
+      <c r="H10">
+        <v>2.8889960340169534</v>
+      </c>
+      <c r="I10">
+        <v>1.7633227677230631E-9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>0.26577672103244981</v>
+      </c>
+      <c r="C11">
+        <v>9.1599662009929656E-3</v>
+      </c>
+      <c r="D11">
+        <v>7.3359746404164677E-2</v>
+      </c>
+      <c r="E11">
+        <v>4.0195995714306711</v>
+      </c>
+      <c r="F11">
+        <v>1.2517235064459871E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.44937654633895496</v>
+      </c>
+      <c r="H11">
+        <v>2.4422175341009207</v>
+      </c>
+      <c r="I11">
+        <v>5.482915829852193E-15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="str">
+        <f>IF(NOT(ISNUMBER(FIND("E",B2))),_xlfn.CONCAT(ROUND(B2,2), " ± ", ROUND(B8,2)),_xlfn.CONCAT(LEFT(B2,4),RIGHT(B2,4), " ± ",LEFT(B8,4),RIGHT(B8,4)))</f>
+        <v>49.3 ± 0.75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ref="C13:I13" si="0">IF(NOT(ISNUMBER(FIND("E",D2))),_xlfn.CONCAT(ROUND(D2,2), " ± ", ROUND(D8,2)),_xlfn.CONCAT(LEFT(D2,4),RIGHT(D2,4), " ± ",LEFT(D8,4),RIGHT(D8,4)))</f>
+        <v>0.19 ± 0.03</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>20.81 ± 5.58</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>3.08E-14 ± 6.85E-15</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.19 ± 0.04</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.15 ± 0.04</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.06 ± 0.06</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" ref="B14:I16" si="1">IF(NOT(ISNUMBER(FIND("E",B3))),_xlfn.CONCAT(ROUND(B3,2), " ± ", ROUND(B9,2)),_xlfn.CONCAT(LEFT(B3,4),RIGHT(B3,4), " ± ",LEFT(B9,4),RIGHT(B9,4)))</f>
+        <v>49.56 ± 0.19</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.02 ± 0.01</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.1 ± 0.1</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>19.73 ± 4.45</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.9 ± 0.44</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.81 ± 0.45</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="1"/>
+        <v>50.61 ± 0.39</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>0.03 ± 0.02</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>0.15 ± 0.07</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>16.65 ± 3.04</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>1.27 ± 0.89</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>3.4 ± 2.89</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v>3.50E-09 ± 1.76E-09</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="1"/>
+        <v>50.39 ± 0.27</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>0.02 ± 0.01</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>0.13 ± 0.07</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>17.23 ± 4.02</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>0.01 ± 0.01</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>0.53 ± 0.45</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>2.68 ± 2.44</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>2.76E-14 ± 5.48E-15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>